<commit_message>
Small fixes- fix vidToFrames.py on some machines, syntax error in Salient Trace 18
</commit_message>
<xml_diff>
--- a/Finished POI Spreadsheets/18 POI Finished.xlsx
+++ b/Finished POI Spreadsheets/18 POI Finished.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qwe\Documents\vr-viewport-analysis\Finished POI Spreadsheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C14EBF8-E7D0-40A3-A69B-99A5437CFFEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1422" yWindow="786" windowWidth="21600" windowHeight="11148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Frame</t>
   </si>
@@ -26,9 +35,6 @@
   </si>
   <si>
     <t>Y1</t>
-  </si>
-  <si>
-    <t>User may look anywhere</t>
   </si>
   <si>
     <t xml:space="preserve">From frame 1021 to 1501, </t>
@@ -43,57 +49,66 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -283,24 +298,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="21.57"/>
-    <col customWidth="1" min="6" max="6" width="23.14"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -317,251 +337,249 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1886.0</v>
+        <v>1886</v>
       </c>
       <c r="C2" s="1">
-        <v>1050.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1021.0</v>
+        <v>1021</v>
       </c>
       <c r="B3" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C3" s="1">
-        <v>1200.0</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1051</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>1051.0</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3000.0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1400.0</v>
-      </c>
-      <c r="F4" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1081</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>1081.0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3000.0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1400.0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>1111.0</v>
+        <v>1111</v>
       </c>
       <c r="B6" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C6" s="1">
-        <v>1200.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1141.0</v>
+        <v>1141</v>
       </c>
       <c r="B7" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C7" s="1">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>1171.0</v>
+        <v>1171</v>
       </c>
       <c r="B8" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C8" s="1">
-        <v>1700.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>1201.0</v>
+        <v>1201</v>
       </c>
       <c r="B9" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C9" s="1">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>121.0</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C10" s="1">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="D10" s="1">
-        <v>2200.0</v>
+        <v>2200</v>
       </c>
       <c r="E10" s="1">
-        <v>1850.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>1231.0</v>
+        <v>1231</v>
       </c>
       <c r="B11" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C11" s="1">
-        <v>1400.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>1261.0</v>
+        <v>1261</v>
       </c>
       <c r="B12" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C12" s="1">
-        <v>1500.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>1291.0</v>
+        <v>1291</v>
       </c>
       <c r="B13" s="1">
-        <v>2900.0</v>
+        <v>2900</v>
       </c>
       <c r="C13" s="1">
-        <v>1590.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>1321.0</v>
+        <v>1321</v>
       </c>
       <c r="B14" s="1">
-        <v>2900.0</v>
+        <v>2900</v>
       </c>
       <c r="C14" s="1">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>1351.0</v>
+        <v>1351</v>
       </c>
       <c r="B15" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C15" s="1">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>1381.0</v>
+        <v>1381</v>
       </c>
       <c r="B16" s="1">
-        <v>2850.0</v>
+        <v>2850</v>
       </c>
       <c r="C16" s="1">
-        <v>1650.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>1411.0</v>
+        <v>1411</v>
       </c>
       <c r="B17" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C17" s="1">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>1441.0</v>
+        <v>1441</v>
       </c>
       <c r="B18" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C18" s="1">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>1471.0</v>
+        <v>1471</v>
       </c>
       <c r="B19" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="C19" s="1">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>1501.0</v>
+        <v>1501</v>
       </c>
       <c r="B20" s="1">
-        <v>2950.0</v>
+        <v>2950</v>
       </c>
       <c r="C20" s="1">
-        <v>1500.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>151.0</v>
+        <v>151</v>
       </c>
       <c r="B21" s="1">
-        <v>2200.0</v>
+        <v>2200</v>
       </c>
       <c r="C21" s="1">
-        <v>1885.0</v>
+        <v>1885</v>
       </c>
       <c r="D21" s="1">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="E21" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>